<commit_message>
Changes to be committed: 	new file:   Results/combined_data.xlsx 	modified:   Results/extracted_table.xlsx 	modified:   VRU Headform
</commit_message>
<xml_diff>
--- a/Results/extracted_table.xlsx
+++ b/Results/extracted_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,154 +441,171 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 2</t>
+          <t>Unnamed: 4</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 3</t>
+          <t>Unnamed: 16</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 4</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 5</t>
+          <t>Unnamed: 19</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PREDICTION</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Nr of points</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Blue</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>Points</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Predicted headform score (excluding blue points)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>D Green</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>29</v>
+      </c>
+      <c r="D4" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>VERIFICATION</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>101</v>
+      </c>
+      <c r="D5" t="n">
+        <v>75.75</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Testpoint</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Prediction</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>44</v>
+      </c>
+      <c r="D6" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>7,2</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>13,-2</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Yellow</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>26</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>9,1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Orange</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Default Red</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>11,7</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Red</t>
-        </is>
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
       </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2,6</t>
+          <t>Predicted headform score (excluding blue points)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Yellow</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>232</v>
+      </c>
+      <c r="D11" t="n">
+        <v>131.75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>VERIFICATION</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>